<commit_message>
Add basic editing, loading, and saving of all dataset metadata.
</commit_message>
<xml_diff>
--- a/mapclientplugins/generatesdsstep/resources/submission.xlsx
+++ b/mapclientplugins/generatesdsstep/resources/submission.xlsx
@@ -1,64 +1,97 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hsor001/Projects/musculoskeletal/mapclientplugins/sparc/mapclientplugins.generatesds/mapclientplugins/generatesdsstep/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98D3307-FD25-B349-8C11-328A6C6A170F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="18840" windowHeight="12120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Submission Item</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Consortium data standard</t>
+  </si>
+  <si>
+    <t>Name of the consortium data standard under which this dataset will be processed. Examples: SPARC, HEAL</t>
+  </si>
+  <si>
+    <t>SPARC, SPARC-2, VESPA, REVA, HORNET, REJOIN-HEAL, EXTERNAL</t>
+  </si>
+  <si>
+    <t>Award number</t>
+  </si>
+  <si>
+    <t>Primary grant number supporting the milestone.</t>
+  </si>
+  <si>
+    <t>Milestone achieved</t>
+  </si>
+  <si>
+    <t>From milestones supplied to NIH</t>
+  </si>
+  <si>
+    <t>Milestone completion date</t>
+  </si>
+  <si>
+    <t>Date of milestone completion. Refer to your consortium for detailed information.</t>
+  </si>
+  <si>
+    <t>Funding consortium</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="14"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -79,67 +112,45 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -198,8 +209,24 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -487,107 +514,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col width="30.77" customWidth="1" style="6" min="1" max="1"/>
-    <col width="42.68" customWidth="1" style="7" min="2" max="2"/>
-    <col width="28.25" customWidth="1" style="6" min="3" max="3"/>
+    <col min="1" max="1" width="30.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18" customHeight="1" s="8">
-      <c r="A1" s="9" t="inlineStr">
-        <is>
-          <t>Submission Item</t>
-        </is>
-      </c>
-      <c r="B1" s="9" t="inlineStr">
-        <is>
-          <t>Definition</t>
-        </is>
-      </c>
-      <c r="C1" s="9" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
+    <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2" ht="50.25" customHeight="1" s="8">
-      <c r="A2" s="10" t="inlineStr">
-        <is>
-          <t>Consortium data standard</t>
-        </is>
-      </c>
-      <c r="B2" s="11" t="inlineStr">
-        <is>
-          <t>Name of the consortium data standard under which this dataset will be processed. Examples: SPARC, HEAL</t>
-        </is>
+    <row r="2" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="3" ht="33.75" customHeight="1" s="8">
-      <c r="A3" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Funding consortium </t>
-        </is>
-      </c>
-      <c r="B3" s="11" t="inlineStr">
-        <is>
-          <t>SPARC, SPARC-2, VESPA, REVA, HORNET, REJOIN-HEAL, EXTERNAL</t>
-        </is>
+    <row r="3" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="4" ht="33.75" customHeight="1" s="8">
-      <c r="A4" s="10" t="inlineStr">
-        <is>
-          <t>Award number</t>
-        </is>
-      </c>
-      <c r="B4" s="11" t="inlineStr">
-        <is>
-          <t>Primary grant number supporting the milestone.</t>
-        </is>
+    <row r="4" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" ht="17.25" customHeight="1" s="8">
-      <c r="A5" s="10" t="inlineStr">
-        <is>
-          <t>Milestone achieved</t>
-        </is>
-      </c>
-      <c r="B5" s="11" t="inlineStr">
-        <is>
-          <t>From milestones supplied to NIH</t>
-        </is>
+    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="6" ht="33.75" customHeight="1" s="8">
-      <c r="A6" s="10" t="inlineStr">
-        <is>
-          <t>Milestone completion date</t>
-        </is>
-      </c>
-      <c r="B6" s="11" t="inlineStr">
-        <is>
-          <t>Date of milestone completion. Refer to your consortium for detailed information.</t>
-        </is>
+    <row r="6" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="7" ht="17.25" customHeight="1" s="8"/>
-    <row r="8" ht="17.25" customHeight="1" s="8"/>
-    <row r="9" ht="17.25" customHeight="1" s="8"/>
+    <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>